<commit_message>
add IHC specific enums
</commit_message>
<xml_diff>
--- a/template_examples/tissue_slide_template.xlsx
+++ b/template_examples/tissue_slide_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C742A408-1574-7947-A3AF-DD9990855E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA0345F-3B48-B84E-B2AB-8EC33A44C575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28480" windowHeight="11480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -937,7 +937,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="274">
   <si>
     <t>#t</t>
   </si>
@@ -1350,6 +1350,9 @@
     <t>WES</t>
   </si>
   <si>
+    <t>IHC</t>
+  </si>
+  <si>
     <t>MDA_Wistuba</t>
   </si>
   <si>
@@ -1647,6 +1650,9 @@
     <t>Cells per Vial</t>
   </si>
   <si>
+    <t>Slides</t>
+  </si>
+  <si>
     <t>RT</t>
   </si>
   <si>
@@ -1686,83 +1692,80 @@
     <t>Sample received from CIMAC</t>
   </si>
   <si>
-    <t>Arm_ Z</t>
+    <t>TTTPP801</t>
+  </si>
+  <si>
+    <t>TRIALGROUP 1</t>
+  </si>
+  <si>
+    <t>BIOBANK 1</t>
+  </si>
+  <si>
+    <t>CTTTP08T1.00</t>
   </si>
   <si>
     <t>A1</t>
   </si>
   <si>
-    <t>Slides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass </t>
-  </si>
-  <si>
-    <t>Arm_ A</t>
+    <t>TTTPP802</t>
+  </si>
+  <si>
+    <t>TRIALGROUP 2</t>
+  </si>
+  <si>
+    <t>CTTTP08T2.00</t>
   </si>
   <si>
     <t>A2</t>
   </si>
   <si>
-    <t>Arm_ B</t>
+    <t>TTTPP803</t>
+  </si>
+  <si>
+    <t>TRIALGROUP 3</t>
+  </si>
+  <si>
+    <t>CTTTP08T3.00</t>
   </si>
   <si>
     <t>A3</t>
   </si>
   <si>
-    <t>Off-study</t>
-  </si>
-  <si>
-    <t>Arm_ C</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 1</t>
-  </si>
-  <si>
-    <t>BIOBANK 1</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 2</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 3</t>
+    <t>TTTPP901</t>
   </si>
   <si>
     <t>TRIALGROUP 4</t>
   </si>
   <si>
+    <t>CTTTP09T1.00</t>
+  </si>
+  <si>
     <t>A4</t>
   </si>
   <si>
-    <t>TTTPP801</t>
-  </si>
-  <si>
-    <t>TTTPP802</t>
-  </si>
-  <si>
-    <t>TTTPP803</t>
-  </si>
-  <si>
-    <t>TTTPP901</t>
-  </si>
-  <si>
-    <t>CTTTP08T1.00</t>
-  </si>
-  <si>
-    <t>CTTTP08T2.00</t>
-  </si>
-  <si>
-    <t>CTTTP08T3.00</t>
-  </si>
-  <si>
-    <t>CTTTP09T1.00</t>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>TrackN</t>
+  </si>
+  <si>
+    <t>AccN</t>
+  </si>
+  <si>
+    <t>ship from</t>
+  </si>
+  <si>
+    <t>ship to</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id_slide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1781,24 +1784,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1873,7 +1858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1890,8 +1875,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2232,7 +2218,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2240,7 +2228,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2249,131 +2237,159 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C2" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C5" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C11" s="6">
+        <v>37174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C12" s="6">
+        <v>37539</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -3389,7 +3405,7 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"Olink,WES,Not Reported,Other"</formula1>
+      <formula1>"Olink,WES,IHC,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"MDA_Wistuba,MDA_Bernatchez,MDA_Al-Atrash,MSSM_Gnjatic,MSSM_Rahman,MSSM_Kim-Schulze,MSSM_Bongers,DFCI_Wu,DFCI_Hodi,Broad_Cibulskis,Stanf_Maecker,Stanf_Bendall,Nationwide Children's Hospital,Adaptive Biotechnologies,FNLCR_MoCha,Not Reported,Other"</formula1>
@@ -3416,8 +3432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3539,7 +3555,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3547,46 +3563,46 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>265</v>
+        <v>174</v>
+      </c>
+      <c r="E3" t="s">
+        <v>251</v>
       </c>
       <c r="F3" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G3" t="s">
-        <v>260</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>269</v>
+        <v>253</v>
+      </c>
+      <c r="H3" t="s">
+        <v>254</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="K3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="P3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="Q3">
         <v>4</v>
@@ -3595,28 +3611,28 @@
         <v>3</v>
       </c>
       <c r="S3" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="V3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="W3" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="X3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Y3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -3624,46 +3640,46 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F4" t="s">
+        <v>257</v>
+      </c>
+      <c r="G4" t="s">
         <v>253</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="F4" t="s">
-        <v>261</v>
-      </c>
-      <c r="G4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>270</v>
+      <c r="H4" t="s">
+        <v>258</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="K4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="P4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="Q4">
         <v>4</v>
@@ -3672,28 +3688,28 @@
         <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="T4">
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="V4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="W4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="X4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Y4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3701,46 +3717,46 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>267</v>
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>260</v>
       </c>
       <c r="F5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H5" t="s">
         <v>262</v>
-      </c>
-      <c r="G5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="K5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="P5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -3749,28 +3765,28 @@
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="V5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="W5" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="X5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Y5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3778,37 +3794,37 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>258</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>268</v>
+        <v>177</v>
+      </c>
+      <c r="E6" t="s">
+        <v>264</v>
       </c>
       <c r="F6" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G6" t="s">
-        <v>260</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>272</v>
+        <v>253</v>
+      </c>
+      <c r="H6" t="s">
+        <v>266</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="K6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -3817,7 +3833,7 @@
         <v>133</v>
       </c>
       <c r="P6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -3826,22 +3842,22 @@
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="T6">
         <v>0</v>
       </c>
       <c r="U6" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="V6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="W6" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="X6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Y6" t="s">
         <v>133</v>
@@ -4855,8 +4871,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P202" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>"Whole Blood,Plasma,PBMC,Buffy Coat,Bone Marrow Mononuclear Cell,Supernatant,Cell Pellet,H&amp;E-Stained Fixed Tissue Slide Specimen,Fixed Slide,Tissue Scroll,FFPE Punch,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U202 S3:S202" xr:uid="{00000000-0002-0000-0100-000007000000}">
-      <formula1>"Microliters,Milliliters,Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S202 U3:U202" xr:uid="{00000000-0002-0000-0100-000007000000}">
+      <formula1>"Microliters,Milliliters,Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Slides,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V202" xr:uid="{00000000-0002-0000-0100-000009000000}">
       <formula1>"RT,4oC,(-20)oC,(-80)oC,LN,Not Reported,Other"</formula1>
@@ -5493,55 +5509,55 @@
         <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="O2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Q2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="R2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="S2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="T2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
@@ -5552,55 +5568,55 @@
         <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="P3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Q3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="R3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="S3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="T3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
@@ -5608,58 +5624,58 @@
         <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K4" t="s">
         <v>133</v>
       </c>
       <c r="L4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="O4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="Q4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="R4" t="s">
         <v>133</v>
       </c>
       <c r="S4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="T4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
@@ -5667,49 +5683,49 @@
         <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
       </c>
       <c r="H5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K5" t="s">
         <v>134</v>
       </c>
       <c r="L5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="Q5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="R5" t="s">
         <v>134</v>
@@ -5725,38 +5741,41 @@
       <c r="B6" t="s">
         <v>122</v>
       </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F6" t="s">
         <v>133</v>
       </c>
       <c r="H6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="L6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="O6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="P6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="Q6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="S6" t="s">
         <v>134</v>
@@ -5770,34 +5789,34 @@
         <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F7" t="s">
         <v>134</v>
       </c>
       <c r="H7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="P7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="Q7" t="s">
         <v>133</v>
@@ -5808,31 +5827,31 @@
         <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M8" t="s">
         <v>133</v>
       </c>
       <c r="N8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="O8" t="s">
-        <v>133</v>
+        <v>237</v>
       </c>
       <c r="P8" t="s">
-        <v>133</v>
+        <v>237</v>
       </c>
       <c r="Q8" t="s">
         <v>134</v>
@@ -5843,31 +5862,31 @@
         <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M9" t="s">
         <v>134</v>
       </c>
       <c r="N9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="O9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
@@ -5875,22 +5894,28 @@
         <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J10" t="s">
         <v>133</v>
       </c>
       <c r="L10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N10" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="O10" t="s">
+        <v>134</v>
+      </c>
+      <c r="P10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
@@ -5898,22 +5923,22 @@
         <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J11" t="s">
         <v>134</v>
       </c>
       <c r="L11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="N11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
@@ -5921,19 +5946,19 @@
         <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="L12" t="s">
         <v>133</v>
       </c>
       <c r="N12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
@@ -5941,13 +5966,13 @@
         <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H13" t="s">
         <v>134</v>
       </c>
       <c r="I13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L13" t="s">
         <v>134</v>
@@ -5961,10 +5986,10 @@
         <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="N14" t="s">
         <v>134</v>
@@ -5975,10 +6000,10 @@
         <v>131</v>
       </c>
       <c r="D15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I15" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.2">
@@ -5986,10 +6011,10 @@
         <v>132</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
@@ -6000,7 +6025,7 @@
         <v>133</v>
       </c>
       <c r="I17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
@@ -6011,22 +6036,22 @@
         <v>134</v>
       </c>
       <c r="I18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add prism tests for template.type=tissue_slide
</commit_message>
<xml_diff>
--- a/template_examples/tissue_slide_template.xlsx
+++ b/template_examples/tissue_slide_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA0345F-3B48-B84E-B2AB-8EC33A44C575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0690DD-4908-FA44-A569-D00F12BF7E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1765,7 +1765,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1784,6 +1784,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1872,11 +1878,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2218,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2232,10 +2238,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2343,7 +2349,7 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>37174</v>
       </c>
     </row>
@@ -2354,7 +2360,7 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>37539</v>
       </c>
     </row>
@@ -3432,8 +3438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3443,37 +3449,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -3717,10 +3723,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E5" t="s">
         <v>260</v>
@@ -3794,10 +3800,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
         <v>264</v>

</xml_diff>

<commit_message>
update templates' receiving party
</commit_message>
<xml_diff>
--- a/template_examples/tissue_slide_template.xlsx
+++ b/template_examples/tissue_slide_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0690DD-4908-FA44-A569-D00F12BF7E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A530DA-A555-E54F-A857-A5758ADDBC77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="1780" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -176,7 +176,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -564,11 +564,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>E4412 or 10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>E4412</t>
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E4412 or 10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -581,7 +607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -594,7 +620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -607,7 +633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -620,7 +646,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S1400I</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -633,7 +672,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S1400I</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -646,7 +698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -659,7 +711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -672,7 +724,150 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E4412</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000010000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>EAY131-Z1D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000011000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E4412</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000012000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>EAY131-Z1D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000013000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E4412</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000014000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000015000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E4412</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000016000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000017000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E4412</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000018000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000019000000}">
       <text>
         <r>
           <rPr>
@@ -685,20 +880,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>E4412</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -711,98 +906,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>E4412</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>S1400I</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>E4412</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Z1D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000011000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>E4412</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000012000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Z1D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000013000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>E4412</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000014000000}">
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -815,59 +945,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000015000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>E4412</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000016000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>E4412</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000017000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>S1400I</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000018000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>S1400I</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000019000000}">
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000020000000}">
       <text>
         <r>
           <rPr>
@@ -880,7 +971,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001A000000}">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000021000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000022000000}">
       <text>
         <r>
           <rPr>
@@ -893,7 +997,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001B000000}">
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000023000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000024000000}">
       <text>
         <r>
           <rPr>
@@ -906,7 +1023,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001C000000}">
+    <comment ref="H21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000025000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000026000000}">
       <text>
         <r>
           <rPr>
@@ -919,16 +1049,107 @@
         </r>
       </text>
     </comment>
-    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00001D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>10021</t>
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000027000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000028000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000029000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00002A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00002B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00002C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00002D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10026</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00002E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9204</t>
         </r>
       </text>
     </comment>
@@ -937,7 +1158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="294">
   <si>
     <t>#t</t>
   </si>
@@ -1353,6 +1574,12 @@
     <t>IHC</t>
   </si>
   <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>ELISA</t>
+  </si>
+  <si>
     <t>MDA_Wistuba</t>
   </si>
   <si>
@@ -1380,6 +1607,9 @@
     <t>DFCI_Hodi</t>
   </si>
   <si>
+    <t>DFCI_Severgnini</t>
+  </si>
+  <si>
     <t>Broad_Cibulskis</t>
   </si>
   <si>
@@ -1461,49 +1691,88 @@
     <t>On_Treatment</t>
   </si>
   <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Relapse</t>
+  </si>
+  <si>
+    <t>Day_8</t>
+  </si>
+  <si>
+    <t>Cycle_2_Day_1</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>End_of_Treatment</t>
+  </si>
+  <si>
+    <t>Not_reported</t>
+  </si>
+  <si>
+    <t>Arm_A</t>
+  </si>
+  <si>
+    <t>Arm_B</t>
+  </si>
+  <si>
+    <t>Arm_C</t>
+  </si>
+  <si>
+    <t>Arm_D</t>
+  </si>
+  <si>
+    <t>Arm_E</t>
+  </si>
+  <si>
+    <t>Arm_F</t>
+  </si>
+  <si>
+    <t>Arm_G</t>
+  </si>
+  <si>
+    <t>Arm_H</t>
+  </si>
+  <si>
+    <t>Arm_I</t>
+  </si>
+  <si>
+    <t>Arm_X</t>
+  </si>
+  <si>
+    <t>Arm_Y</t>
+  </si>
+  <si>
     <t>Arm_Z</t>
   </si>
   <si>
-    <t>Arm_A</t>
-  </si>
-  <si>
-    <t>Arm_B</t>
-  </si>
-  <si>
-    <t>Arm_C</t>
-  </si>
-  <si>
-    <t>Arm_Y</t>
-  </si>
-  <si>
-    <t>Arm_D</t>
-  </si>
-  <si>
-    <t>Arm_E</t>
-  </si>
-  <si>
-    <t>Arm_F</t>
-  </si>
-  <si>
-    <t>Arm_X</t>
-  </si>
-  <si>
-    <t>Arm_G</t>
-  </si>
-  <si>
-    <t>Arm_H</t>
-  </si>
-  <si>
-    <t>Arm_I</t>
-  </si>
-  <si>
     <t>Arm_1</t>
   </si>
   <si>
     <t>Arm_2</t>
   </si>
   <si>
-    <t>Z1D</t>
+    <t>EAY131-Z1D</t>
   </si>
   <si>
     <t>NSCLC_A</t>
@@ -1521,6 +1790,18 @@
     <t>CRC_B</t>
   </si>
   <si>
+    <t>Dose_A</t>
+  </si>
+  <si>
+    <t>Dose_B</t>
+  </si>
+  <si>
+    <t>Dose_C</t>
+  </si>
+  <si>
+    <t>Dose_D</t>
+  </si>
+  <si>
     <t>Tumor Tissue</t>
   </si>
   <si>
@@ -1692,6 +1973,24 @@
     <t>Sample received from CIMAC</t>
   </si>
   <si>
+    <t>test_prism_trial_id_slide</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>TrackN</t>
+  </si>
+  <si>
+    <t>AccN</t>
+  </si>
+  <si>
+    <t>ship from</t>
+  </si>
+  <si>
+    <t>ship to</t>
+  </si>
+  <si>
     <t>TTTPP801</t>
   </si>
   <si>
@@ -1741,24 +2040,6 @@
   </si>
   <si>
     <t>A4</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>TrackN</t>
-  </si>
-  <si>
-    <t>AccN</t>
-  </si>
-  <si>
-    <t>ship from</t>
-  </si>
-  <si>
-    <t>ship to</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_slide</t>
   </si>
 </sst>
 </file>
@@ -1878,11 +2159,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2224,8 +2505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2238,10 +2519,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2251,7 +2532,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2262,7 +2543,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2295,7 +2576,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2306,7 +2587,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2317,7 +2598,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2328,7 +2609,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2349,7 +2630,7 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>37174</v>
       </c>
     </row>
@@ -2360,7 +2641,7 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>37539</v>
       </c>
     </row>
@@ -2372,7 +2653,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2383,7 +2664,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2394,7 +2675,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
@@ -3411,10 +3692,10 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"Olink,WES,IHC,Not Reported,Other"</formula1>
+      <formula1>"Olink,WES,IHC,CyTOF,ELISA"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"MDA_Wistuba,MDA_Bernatchez,MDA_Al-Atrash,MSSM_Gnjatic,MSSM_Rahman,MSSM_Kim-Schulze,MSSM_Bongers,DFCI_Wu,DFCI_Hodi,Broad_Cibulskis,Stanf_Maecker,Stanf_Bendall,Nationwide Children's Hospital,Adaptive Biotechnologies,FNLCR_MoCha,Not Reported,Other"</formula1>
+      <formula1>"MDA_Wistuba,MDA_Bernatchez,MDA_Al-Atrash,MSSM_Gnjatic,MSSM_Rahman,MSSM_Kim-Schulze,MSSM_Bongers,DFCI_Wu,DFCI_Hodi,DFCI_Severgnini,Broad_Cibulskis,Stanf_Maecker,Stanf_Bendall,Nationwide Children's Hospital,Adaptive Biotechnologies,FNLCR_MoCha"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"FEDEX,USPS,UPS,Inter-Site Delivery"</formula1>
@@ -3439,7 +3720,7 @@
   <dimension ref="A1:Z202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3449,37 +3730,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -3569,46 +3850,46 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="F3" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="G3" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="H3" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
       <c r="K3" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="L3" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="M3" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="P3" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="Q3">
         <v>4</v>
@@ -3617,22 +3898,22 @@
         <v>3</v>
       </c>
       <c r="S3" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="V3" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="W3" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="X3" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="Y3" t="s">
         <v>133</v>
@@ -3646,46 +3927,46 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>256</v>
+        <v>282</v>
       </c>
       <c r="F4" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="G4" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="H4" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="K4" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="L4" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="M4" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="P4" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="Q4">
         <v>4</v>
@@ -3694,22 +3975,22 @@
         <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="T4">
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="V4" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="W4" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="X4" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="Y4" t="s">
         <v>133</v>
@@ -3723,46 +4004,46 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="F5" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="G5" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="K5" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="L5" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="M5" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="P5" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -3771,22 +4052,22 @@
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="V5" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="W5" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="X5" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="Y5" t="s">
         <v>133</v>
@@ -3800,37 +4081,37 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="E6" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c r="F6" t="s">
-        <v>265</v>
+        <v>291</v>
       </c>
       <c r="G6" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="H6" t="s">
-        <v>266</v>
+        <v>292</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>267</v>
+        <v>293</v>
       </c>
       <c r="K6" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="L6" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="M6" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -3839,7 +4120,7 @@
         <v>133</v>
       </c>
       <c r="P6" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -3848,22 +4129,22 @@
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="T6">
         <v>0</v>
       </c>
       <c r="U6" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="V6" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="W6" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="X6" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="Y6" t="s">
         <v>133</v>
@@ -4857,10 +5138,10 @@
   </mergeCells>
   <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C202" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>"Baseline,Pre_Day_1_Cycle_2,Restaging,Off_study,Cycle_2_Week_3,Cycle_4_Week_7,Cycle_5_Week_9,Progression,Cycle_3,End_of_treatment,On_Treatment,Other"</formula1>
+      <formula1>"Baseline,Pre_Day_1_Cycle_2,Restaging,Off_study,Cycle_2_Week_3,Cycle_4_Week_7,Cycle_5_Week_9,Progression,Cycle_3,End_of_treatment,On_Treatment,Response,Relapse,Day_8,Cycle_2_Day_1,T0,T1,T2,T3,T4,T5,T6,End_of_Treatment,Progression,Other,Not_reported"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D202" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>"Arm_Z,Arm_A,Arm_B,Arm_C,Arm_Y,Arm_D,Arm_E,Arm_F,Arm_X,Arm_G,Arm_H,Arm_I,Arm_1,Arm_2,Z1D,NSCLC_A,NSCLC_B,NSCLC_C,CRC_A,CRC_B"</formula1>
+      <formula1>"Arm_A,Arm_B,Arm_C,Arm_D,Arm_E,Arm_F,Arm_G,Arm_H,Arm_I,Arm_X,Arm_Y,Arm_Z,Arm_1,Arm_2,EAY131-Z1D,NSCLC_A,NSCLC_B,NSCLC_C,CRC_A,CRC_B,Dose_A,Dose_B,Dose_C,Dose_D,Other,Not_reported"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K202" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Lymph Node,Stool,Not Reported,Other"</formula1>
@@ -5439,7 +5720,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:T21"/>
+  <dimension ref="B1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5515,55 +5796,55 @@
         <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I2" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="J2" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="K2" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="L2" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="M2" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="N2" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="O2" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="P2" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="Q2" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="R2" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="S2" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="T2" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
@@ -5574,55 +5855,55 @@
         <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="I3" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="J3" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="K3" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="L3" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="M3" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="N3" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="O3" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="P3" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="Q3" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="R3" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="S3" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="T3" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
@@ -5633,55 +5914,55 @@
         <v>137</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I4" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="J4" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="K4" t="s">
         <v>133</v>
       </c>
       <c r="L4" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="M4" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="N4" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="O4" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="P4" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="Q4" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="R4" t="s">
         <v>133</v>
       </c>
       <c r="S4" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="T4" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
@@ -5689,49 +5970,49 @@
         <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F5" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
       </c>
       <c r="H5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I5" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="J5" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="K5" t="s">
         <v>134</v>
       </c>
       <c r="L5" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="M5" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="N5" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="O5" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="P5" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="Q5" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="R5" t="s">
         <v>134</v>
@@ -5748,40 +6029,40 @@
         <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F6" t="s">
         <v>133</v>
       </c>
       <c r="H6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="J6" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="L6" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="M6" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="N6" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="O6" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="P6" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="Q6" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="S6" t="s">
         <v>134</v>
@@ -5795,34 +6076,34 @@
         <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F7" t="s">
         <v>134</v>
       </c>
       <c r="H7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="I7" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="J7" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="L7" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="M7" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="N7" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="O7" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="P7" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="Q7" t="s">
         <v>133</v>
@@ -5833,31 +6114,31 @@
         <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="I8" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="J8" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="L8" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="M8" t="s">
         <v>133</v>
       </c>
       <c r="N8" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="O8" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="P8" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="Q8" t="s">
         <v>134</v>
@@ -5868,25 +6149,25 @@
         <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="I9" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="J9" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="L9" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="M9" t="s">
         <v>134</v>
       </c>
       <c r="N9" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="O9" t="s">
         <v>133</v>
@@ -5900,22 +6181,22 @@
         <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H10" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I10" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="J10" t="s">
         <v>133</v>
       </c>
       <c r="L10" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="N10" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="O10" t="s">
         <v>134</v>
@@ -5929,22 +6210,22 @@
         <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H11" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="I11" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="J11" t="s">
         <v>134</v>
       </c>
       <c r="L11" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="N11" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
@@ -5952,19 +6233,19 @@
         <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H12" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="I12" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="L12" t="s">
         <v>133</v>
       </c>
       <c r="N12" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
@@ -5972,13 +6253,13 @@
         <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H13" t="s">
-        <v>134</v>
+        <v>177</v>
       </c>
       <c r="I13" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="L13" t="s">
         <v>134</v>
@@ -5992,10 +6273,13 @@
         <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>152</v>
+      </c>
+      <c r="H14" t="s">
+        <v>178</v>
       </c>
       <c r="I14" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="N14" t="s">
         <v>134</v>
@@ -6006,10 +6290,13 @@
         <v>131</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>153</v>
+      </c>
+      <c r="H15" t="s">
+        <v>179</v>
       </c>
       <c r="I15" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.2">
@@ -6017,10 +6304,13 @@
         <v>132</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>154</v>
+      </c>
+      <c r="H16" t="s">
+        <v>180</v>
       </c>
       <c r="I16" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
@@ -6028,36 +6318,96 @@
         <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>155</v>
+      </c>
+      <c r="H17" t="s">
+        <v>181</v>
       </c>
       <c r="I17" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>134</v>
       </c>
-      <c r="D18" t="s">
+      <c r="H18" t="s">
+        <v>182</v>
+      </c>
+      <c r="I18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>183</v>
+      </c>
+      <c r="I19" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>184</v>
+      </c>
+      <c r="I20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>185</v>
+      </c>
+      <c r="I21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>186</v>
+      </c>
+      <c r="I22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>187</v>
+      </c>
+      <c r="I23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>188</v>
+      </c>
+      <c r="I24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
         <v>134</v>
       </c>
-      <c r="I18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I21" t="s">
-        <v>193</v>
+      <c r="I26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>189</v>
+      </c>
+      <c r="I27" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>